<commit_message>
v0.95 - Snowball+ 설계/운영평가 연계
</commit_message>
<xml_diff>
--- a/paper_templates/Template_Manual.xlsx
+++ b/paper_templates/Template_Manual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\SnowBall\paper_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pythons\snowball\paper_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04932B6B-EF45-47FF-A2D1-99FC98813314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0481ECE-29E4-46A3-90BF-417CE11D0DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5E3EE22-C542-4402-8654-7D4EE4676255}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Prior year control testing documentation rolled forward for reference purposes.</t>
   </si>
@@ -135,46 +135,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>사용자명</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>권한명</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>부서명</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>권한부여일</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>요청자명</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>요청자 부서명</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>승인자명</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>승인일자</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>승인여부</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>사전승인여부</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>결론</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -183,37 +143,11 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="1"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사용자</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Georgia"/>
-        <family val="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
+    <t>Attribute1</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>요청자ID</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>승인자ID</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>권한 요청서 번호</t>
+    <t>Attribute6</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -221,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -319,20 +253,6 @@
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial Unicode MS"/>
-      <family val="1"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -383,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -618,19 +538,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -664,7 +571,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -692,14 +599,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -720,10 +619,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -744,15 +639,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -769,15 +656,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1433,818 +1312,303 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:S31"/>
+  <dimension ref="B1:G31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="5" style="2" customWidth="1"/>
-    <col min="3" max="6" width="15.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" style="3" customWidth="1"/>
-    <col min="9" max="10" width="18.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" style="2" customWidth="1"/>
-    <col min="12" max="14" width="18.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" style="2" customWidth="1"/>
-    <col min="16" max="17" width="20.28515625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="1.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" style="2"/>
-    <col min="21" max="21" width="9.140625" style="2" customWidth="1"/>
-    <col min="22" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="2"/>
+    <col min="9" max="9" width="9.140625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" s="1" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="2:7" s="1" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="35"/>
-    </row>
-    <row r="2" spans="2:19" ht="6" customHeight="1" thickBot="1"/>
-    <row r="3" spans="2:19" ht="24.95" customHeight="1" thickBot="1">
-      <c r="B3" s="36" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="2:7" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="38"/>
-    </row>
-    <row r="4" spans="2:19" s="6" customFormat="1" ht="14.25" thickBot="1">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="2:7" s="6" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="30" t="s">
+      <c r="C4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="O4" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:19">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="11" t="str">
-        <f>IF(N5="", "X", "O")</f>
-        <v>X</v>
-      </c>
-      <c r="P5" s="11" t="str">
-        <f t="shared" ref="P5:P29" si="0">IF(N5-G5&lt;=0, "O", "X")</f>
-        <v>O</v>
-      </c>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="6"/>
-    </row>
-    <row r="6" spans="2:19">
-      <c r="B6" s="13">
+      <c r="C5" s="12"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="11">
         <v>2</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17" t="str">
-        <f>IF(N6="", "X", "O")</f>
-        <v>X</v>
-      </c>
-      <c r="P6" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="2:19">
-      <c r="B7" s="13">
+      <c r="F6" s="15"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="11">
         <v>3</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17" t="str">
-        <f t="shared" ref="O7:O29" si="1">IF(N7="", "X", "O")</f>
-        <v>X</v>
-      </c>
-      <c r="P7" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="18"/>
-    </row>
-    <row r="8" spans="2:19">
-      <c r="B8" s="13">
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="11">
         <v>4</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P8" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="18"/>
-    </row>
-    <row r="9" spans="2:19">
-      <c r="B9" s="13">
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="11">
         <v>5</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P9" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="6"/>
-    </row>
-    <row r="10" spans="2:19">
-      <c r="B10" s="13">
+      <c r="F9" s="15"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="11">
         <v>6</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P10" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="18"/>
-    </row>
-    <row r="11" spans="2:19">
-      <c r="B11" s="13">
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="11">
         <v>7</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P11" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="18"/>
-    </row>
-    <row r="12" spans="2:19">
-      <c r="B12" s="13">
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="11">
         <v>8</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P12" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="18"/>
-    </row>
-    <row r="13" spans="2:19">
-      <c r="B13" s="13">
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="11">
         <v>9</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P13" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="18"/>
-    </row>
-    <row r="14" spans="2:19">
-      <c r="B14" s="13">
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="11">
         <v>10</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P14" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="18"/>
-    </row>
-    <row r="15" spans="2:19">
-      <c r="B15" s="13">
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="11">
         <v>11</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P15" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="18"/>
-    </row>
-    <row r="16" spans="2:19">
-      <c r="B16" s="13">
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="11">
         <v>12</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P16" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="2:18">
-      <c r="B17" s="13">
+      <c r="F16" s="15"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="11">
         <v>13</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P17" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="18"/>
-    </row>
-    <row r="18" spans="2:18">
-      <c r="B18" s="13">
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="11">
         <v>14</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P18" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="18"/>
-    </row>
-    <row r="19" spans="2:18">
-      <c r="B19" s="13">
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="11">
         <v>15</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P19" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="18"/>
-    </row>
-    <row r="20" spans="2:18">
-      <c r="B20" s="13">
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="11">
         <v>16</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P20" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="18"/>
-    </row>
-    <row r="21" spans="2:18">
-      <c r="B21" s="13">
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="11">
         <v>17</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P21" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="18"/>
-    </row>
-    <row r="22" spans="2:18">
-      <c r="B22" s="13">
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="11">
         <v>18</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P22" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="18"/>
-    </row>
-    <row r="23" spans="2:18" ht="15" customHeight="1">
-      <c r="B23" s="13">
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="11">
         <v>19</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P23" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="18"/>
-    </row>
-    <row r="24" spans="2:18" ht="15" customHeight="1">
-      <c r="B24" s="13">
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="11">
         <v>20</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P24" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="18"/>
-    </row>
-    <row r="25" spans="2:18" ht="15" customHeight="1">
-      <c r="B25" s="13">
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="11">
         <v>21</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P25" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="18"/>
-    </row>
-    <row r="26" spans="2:18" ht="15" customHeight="1">
-      <c r="B26" s="13">
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="11">
         <v>22</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P26" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="18"/>
-    </row>
-    <row r="27" spans="2:18">
-      <c r="B27" s="13">
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="11">
         <v>23</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P27" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="18"/>
-    </row>
-    <row r="28" spans="2:18">
-      <c r="B28" s="13">
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="11">
         <v>24</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P28" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="18"/>
-    </row>
-    <row r="29" spans="2:18" ht="13.5" thickBot="1">
-      <c r="B29" s="19">
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="16">
         <v>25</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="P29" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>O</v>
-      </c>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-    </row>
-    <row r="30" spans="2:18" ht="14.45" customHeight="1"/>
-    <row r="31" spans="2:18" s="26" customFormat="1">
-      <c r="B31" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="25"/>
-      <c r="H31" s="27"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:R1"/>
-    <mergeCell ref="B3:R3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2258,7 +1622,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>